<commit_message>
Economy of Building Finalized
added comments on what to do next
</commit_message>
<xml_diff>
--- a/SaveEarth/Assets/Economy/BuildingEconomy.xlsx
+++ b/SaveEarth/Assets/Economy/BuildingEconomy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SaveEarth\SaveEarthFromGlobalWarming\SaveEarth\Assets\Economy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E0C3A0-F516-4E5C-806D-7107BF321C9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{764D6786-CF0D-456D-9D23-AFF6027A3E1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{3C1473EB-D313-427D-84B9-052342A70320}"/>
   </bookViews>
@@ -423,7 +423,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,13 +484,13 @@
         <v>-20</v>
       </c>
       <c r="D3">
-        <v>-25</v>
+        <v>-10</v>
       </c>
       <c r="E3">
-        <v>-35</v>
+        <v>20</v>
       </c>
       <c r="F3">
-        <v>-50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Resources, excel sheets and connections made
</commit_message>
<xml_diff>
--- a/SaveEarth/Assets/Economy/BuildingEconomy.xlsx
+++ b/SaveEarth/Assets/Economy/BuildingEconomy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SaveEarth\SaveEarthFromGlobalWarming\SaveEarth\Assets\Economy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{764D6786-CF0D-456D-9D23-AFF6027A3E1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3978FA2E-4BD1-4F55-B4F0-8C33031EACDD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{3C1473EB-D313-427D-84B9-052342A70320}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>DataID</t>
   </si>
@@ -48,23 +48,35 @@
     <t>Filteration Plant</t>
   </si>
   <si>
-    <t>PO_1</t>
-  </si>
-  <si>
-    <t>PO_2</t>
-  </si>
-  <si>
-    <t>PO_3</t>
-  </si>
-  <si>
-    <t>PO_4</t>
+    <t>cost_prog</t>
+  </si>
+  <si>
+    <t>Wood</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>Stone</t>
+  </si>
+  <si>
+    <t>Metal</t>
+  </si>
+  <si>
+    <t>Pollution</t>
+  </si>
+  <si>
+    <t>pol_prog</t>
+  </si>
+  <si>
+    <t>Cost</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,6 +88,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -104,7 +122,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -420,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35F7D1F4-27E9-408F-9BA0-A0B0276869DF}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,29 +449,38 @@
     <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
+      <c r="C1" t="s">
+        <v>9</v>
       </c>
       <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
+      <c r="E1" t="s">
+        <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -461,19 +488,25 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E2">
-        <v>20</v>
+        <v>200</v>
       </c>
       <c r="F2">
-        <v>40</v>
+        <v>300</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -481,19 +514,25 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>-20</v>
+        <v>200</v>
       </c>
       <c r="D3">
-        <v>-10</v>
+        <v>100</v>
       </c>
       <c r="E3">
+        <v>50</v>
+      </c>
+      <c r="F3">
         <v>20</v>
       </c>
-      <c r="F3">
-        <v>40</v>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -501,19 +540,25 @@
         <v>4</v>
       </c>
       <c r="C4">
-        <v>60</v>
+        <v>300</v>
       </c>
       <c r="D4">
-        <v>140</v>
+        <v>200</v>
       </c>
       <c r="E4">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="F4">
-        <v>400</v>
+        <v>150</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -521,19 +566,25 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <v>-20</v>
+        <v>400</v>
       </c>
       <c r="D5">
-        <v>-50</v>
+        <v>300</v>
       </c>
       <c r="E5">
-        <v>-150</v>
+        <v>200</v>
       </c>
       <c r="F5">
-        <v>-300</v>
+        <v>100</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -541,19 +592,26 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>20</v>
+        <v>150</v>
       </c>
       <c r="D6">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="E6">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="F6">
-        <v>100</v>
+        <v>50</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>